<commit_message>
learning how to make data cloud
</commit_message>
<xml_diff>
--- a/practice_articles.xlsx
+++ b/practice_articles.xlsx
@@ -446,220 +446,220 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>나훈아와 유시민이 불러낸 ‘테스형!’</t>
+          <t>재방송 없다던 '나훈아 콘서트', 중국 사이트서 불법 유통</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.sedaily.com/NewsView/1Z8Z4OC8W8</t>
+          <t>https://biz.chosun.com/site/data/html_dir/2020/10/03/2020100300934.html?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=biz</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>서울경제</t>
+          <t>조선비즈</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F011%2F2020%2F10%2F02%2F3805411.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F366%2F2020%2F10%2F03%2F598144.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>나훈아 스페셜VS기생충…개천절 동시간 방송, 승자는?</t>
+          <t>'나훈아 스페셜' 나훈아 "가수로 54년째…연습만이 살길"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://www.edaily.co.kr/news/newspath.asp?newsid=01312006625928984</t>
+          <t>https://www.news1.kr/articles/?4076175</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>이데일리</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F018%2F2020%2F10%2F02%2F4750188.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F421%2F2020%2F10%2F03%2F4904242.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>주호영 "나훈아씨가 우리 마음 속시원하게 대변"</t>
+          <t>"이번엔 나훈아로" 文비판이라면 나훈아도 정쟁 수단?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://news.mt.co.kr/mtview.php?no=2020100214281626187</t>
+          <t>http://www.mediatoday.co.kr/news/articleView.html?idxno=209591</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>머니투데이</t>
+          <t>미디어오늘</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F008%2F2020%2F10%2F02%2F4478970.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F006%2F2020%2F10%2F03%2F104801.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"KBS, 15년만에 나훈아 컴백시키는데…野, 무대 없다"</t>
+          <t>나훈아와 유시민이 불러낸 ‘테스형!’</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://www.edaily.co.kr/news/newspath.asp?newsid=01498966625928984</t>
+          <t>https://www.sedaily.com/NewsView/1Z8Z4OC8W8</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>이데일리</t>
+          <t>서울경제</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F018%2F2020%2F10%2F02%2F4750262.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F011%2F2020%2F10%2F02%2F3805411.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>나훈아 "검은우산의 의미?" 정치권에도 파장</t>
+          <t>윤평중 “유시민, 권력 결사옹위 위해 궤변…광대 나훈아가 소크라테스에 가깝...</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://www.fntoday.co.kr/news/articleView.html?idxno=234198</t>
+          <t>http://www.munhwa.com/news/view.html?no=20201003MW104009406914</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>파이낸스투데이</t>
+          <t>문화일보</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F5585%2F2020%2F10%2F02%2F55584.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F021%2F2020%2F10%2F03%2F2444422.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>주호영 “나훈아, 우리 마음 대변해…제1야당 숙제 분명해져”</t>
+          <t>나훈아 스페셜VS기생충…개천절 동시간 방송, 승자는?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://www.hani.co.kr/arti/politics/assembly/964223.html</t>
+          <t>http://www.edaily.co.kr/news/newspath.asp?newsid=01312006625928984</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>한겨레</t>
+          <t>이데일리</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F028%2F2020%2F10%2F02%2F2514836.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F018%2F2020%2F10%2F02%2F4750188.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"나훈아, 지친 국민 위로" 정치권도 들썩…野 '소신 발언' 부각</t>
+          <t>주호영 “나훈아, 우리 마음 대변해…제1야당 숙제 분명해져”</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>http://yna.kr/AKR20201001029400001?did=1195m</t>
+          <t>http://www.hani.co.kr/arti/politics/assembly/964223.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>연합뉴스</t>
+          <t>한겨레</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F001%2F2020%2F10%2F01%2F11916973.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F028%2F2020%2F10%2F02%2F2514836.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>나훈아 "국민 위해 목숨 건 대통령 못 봐"…야권 "부끄럽다"</t>
+          <t>‘나훈아쇼’ 이어 ‘트롯전국체전’에 거는 기대 [MK★이슈]</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>http://www.newsis.com/view/?id=NISX20201001_0001184710&amp;cID=10301&amp;pID=10300</t>
+          <t>http://mksports.co.kr/view/2020/1012057/</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>뉴시스</t>
+          <t>MK스포츠</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F003%2F2020%2F10%2F01%2F10105052.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F410%2F2020%2F10%2F03%2F732267.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>“국민이 힘 있으면 위정자가 생길 수 없다” 나훈아에 야권도 들썩</t>
+          <t>[TF 확대경] '나훈아 스페셜', 시청자 찬사가 끊이지 않는 이유?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.chosun.com/politics/politics_general/2020/10/01/DP4NWFDPMZB7ZP6FNKAM4TRMA4/?utm_source=naver&amp;utm_medium=original&amp;utm_campaign=news</t>
+          <t>http://news.tf.co.kr/read/entertain/1816218.htm</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>조선일보</t>
+          <t>더팩트</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F023%2F2020%2F10%2F01%2F3565776.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F629%2F2020%2F10%2F03%2F45020.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>나훈아 발언 화제..."정부 비판" vs "확대 해석"</t>
+          <t>정치권도 뒤흔든 나훈아…"위대한 카리스마""자괴감 들었다"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.ytn.co.kr/_ln/0106_202010012203408768</t>
+          <t>https://news.joins.com/article/olink/23479315</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>YTN</t>
+          <t>중앙일보</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F052%2F2020%2F10%2F01%2F1497320.jpg&amp;type=ofullfill80_80_q75_re2</t>
+          <t>https://search.pstatic.net/common/?src=https%3A%2F%2Fimgnews.pstatic.net%2Fimage%2Forigin%2F025%2F2020%2F10%2F01%2F3039989.jpg&amp;type=ofullfill80_80_q75_re2</t>
         </is>
       </c>
     </row>

</xml_diff>